<commit_message>
#unique changed to #match
Changed #unique over to #match. Changed #unique=false to #match=all in all testing files. Added some more tests for tracking and untracking to cover lines that were previously not covered.
</commit_message>
<xml_diff>
--- a/tests/testing_files/base_source.xlsx
+++ b/tests/testing_files/base_source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparda\Desktop\Moseley Lab\Code\MESSES\tests\testing_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2F446C-4CB2-45D1-A0DB-7CF3511462A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AACDA3-142F-4220-8D5A-70561F816C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="2685" windowWidth="23565" windowHeight="12015" activeTab="1" xr2:uid="{15FD60AA-0CC8-9F4F-B5F4-2B27D5230080}"/>
+    <workbookView xWindow="4155" yWindow="2340" windowWidth="23640" windowHeight="12015" xr2:uid="{15FD60AA-0CC8-9F4F-B5F4-2B27D5230080}"/>
   </bookViews>
   <sheets>
     <sheet name="#convert" sheetId="6" r:id="rId1"/>
@@ -251,13 +251,13 @@
     <t>IC-FTMS_measurement</t>
   </si>
   <si>
-    <t>#unique=false</t>
-  </si>
-  <si>
     <t>#measurement.id.regex</t>
   </si>
   <si>
     <t>r'\(S\)-2-Acetolactate_Glutaric acid_Methylsuccinic acid_MP_NoStd',r'(S)-2-Acetolactate Glutaric acid Methylsuccinic acid'</t>
+  </si>
+  <si>
+    <t>#match=all</t>
   </si>
 </sst>
 </file>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8067F3B6-BC85-4627-B925-1366E7FE6A62}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -648,10 +648,10 @@
         <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -671,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FFFD15-87D9-4AFC-82C0-CA4CE918806E}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>